<commit_message>
Merged PR 17692: BP-5515_Client name is too small to read when Line Up is exported with postin...
BP-5515_Client name is too small to read when Line Up is exported with posting Type as  NSI
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup with Allocation by Affiliate.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup with Allocation by Affiliate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3667881F-A237-40A7-A2B8-33E108D7574C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15351A9C-4F13-4722-BC7D-380376020E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default View" sheetId="7" r:id="rId1"/>
@@ -355,7 +355,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -489,6 +489,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -1818,7 +1821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9:I9"/>
     </sheetView>
@@ -2361,7 +2364,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I11">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A9="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2375,9 +2378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O93"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2:K2"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2480,7 +2483,7 @@
     <row r="6" spans="1:15" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
-      <c r="E6" s="16"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="47"/>
       <c r="G6" s="47"/>
       <c r="H6" s="16"/>
@@ -2956,7 +2959,7 @@
     <mergeCell ref="E3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:K1048576">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Merged PR 17694: BP-5515_Client name is too small to read when Line Up is exported with posting Type as  NSI
BP-5515_Client name is too small to read when Line Up is exported with posting Type as  NSI
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup with Allocation by Affiliate.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup with Allocation by Affiliate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15351A9C-4F13-4722-BC7D-380376020E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861E645-8216-4E80-ABDA-B48960351EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default View" sheetId="7" r:id="rId1"/>
@@ -130,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -225,6 +225,18 @@
       <sz val="12"/>
       <color rgb="FF62819A"/>
       <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF3D5261"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -355,7 +367,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -491,8 +503,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1034,9 +1049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M111"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="46"/>
-      <c r="E6" s="25">
+      <c r="E6" s="52">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
@@ -2378,9 +2393,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2970,6 +2985,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3192,15 +3216,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3208,6 +3223,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3226,14 +3249,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Merged PR 17744: BP-5515_Client name is too small to read when Line Up is exported with posting Type as  NSI
BP-5515_Client name is too small to read when Line Up is exported with posting Type as  NSI
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup with Allocation by Affiliate.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Program Lineup with Allocation by Affiliate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861E645-8216-4E80-ABDA-B48960351EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E409E431-5640-45BA-943D-232A418E0D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default View" sheetId="7" r:id="rId1"/>
@@ -482,6 +482,12 @@
     <xf numFmtId="10" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -502,19 +508,20 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF5F8F8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -577,13 +584,13 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="7"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1049,9 +1056,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M111"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1084,24 +1091,24 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="48">
+      <c r="J2" s="50">
         <f>'Detailed View'!J2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="48"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1121,10 +1128,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
@@ -1149,20 +1156,20 @@
       </c>
     </row>
     <row r="6" spans="2:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="46">
+      <c r="C6" s="48">
         <f>'Detailed View'!C6:D6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="52">
+      <c r="D6" s="48"/>
+      <c r="E6" s="45">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="49">
         <f>'Detailed View'!F6:G6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
@@ -1822,7 +1829,7 @@
     <mergeCell ref="J2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:I1048576">
-    <cfRule type="expression" dxfId="3" priority="21">
+    <cfRule type="expression" dxfId="4" priority="21">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1836,9 +1843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M105"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9:I9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1871,24 +1878,24 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="48">
+      <c r="J2" s="50">
         <f>'Detailed View'!J2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="48"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -1908,10 +1915,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="26" t="s">
         <v>13</v>
       </c>
@@ -1936,20 +1943,20 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="46">
+      <c r="C6" s="48">
         <f>'Detailed View'!C6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="25">
+      <c r="D6" s="48"/>
+      <c r="E6" s="45">
         <f>'Detailed View'!E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="49">
         <f>'Detailed View'!F6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="25">
         <f>'Detailed View'!H6</f>
         <v>0</v>
@@ -1975,16 +1982,16 @@
     <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="G9" s="50" t="s">
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="G9" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
     </row>
     <row r="10" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
@@ -2020,11 +2027,11 @@
     </row>
     <row r="13" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
     </row>
     <row r="14" spans="1:13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
@@ -2050,11 +2057,11 @@
     </row>
     <row r="17" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
     </row>
     <row r="18" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
@@ -2077,11 +2084,11 @@
     </row>
     <row r="21" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
     </row>
     <row r="22" spans="1:5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
@@ -2373,19 +2380,24 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="G9:I9"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="expression" dxfId="2" priority="20">
+  <conditionalFormatting sqref="C1:E5 C7:E1048576 C6:D6">
+    <cfRule type="expression" dxfId="3" priority="21">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I11">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A9="Even"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A6="Even"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2432,22 +2444,22 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="20"/>
       <c r="M2" s="1"/>
       <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2455,12 +2467,12 @@
     </row>
     <row r="4" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
@@ -2468,10 +2480,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="19" t="s">
         <v>13</v>
       </c>
@@ -2496,11 +2508,11 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -2974,7 +2986,7 @@
     <mergeCell ref="E3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:K1048576">
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2985,15 +2997,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -3216,6 +3219,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3223,14 +3235,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{060BAEE3-07B5-4CCF-A906-7A824BD2B0D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3249,6 +3253,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D4F406-DB10-4FCE-90E8-E4689C9E60D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{022D3F0F-7ADC-46CC-B0CC-F40745AEE35B}">
   <ds:schemaRefs>

</xml_diff>